<commit_message>
Update Word generation with template placeholders
- Change generate_docs.py to use python-docx for {{}} placeholder replacement
- Read from 结果.xlsx instead of CSV
- Add date formatting: YYYY年MM月DD日 with time suffix preserved
- Add type field rendering with checkbox options
- Update excel_analyzer.py to export both .xlsx and .csv
- Add font styling: 仿宋_GB2312 小四 for general content
- Business logic verified and working correctly
- Note: Font styling for type field needs further adjustment
</commit_message>
<xml_diff>
--- a/结果.xlsx
+++ b/结果.xlsx
@@ -387,14 +387,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,153 +843,154 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1346,11 +1340,14 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
+    <col min="2" max="2" width="11.7256637168142" customWidth="1"/>
+    <col min="5" max="5" width="13.646017699115" customWidth="1"/>
+    <col min="9" max="9" width="24.2743362831858" customWidth="1"/>
     <col min="10" max="10" width="86.7964601769911" customWidth="1"/>
     <col min="11" max="11" width="55.3097345132743" customWidth="1"/>
   </cols>
@@ -1456,7 +1453,7 @@
       <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2266,6 +2263,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" display="https://mp.weixin.qq.com/s/f5OxcS5VLkwK3vy_04WLHQ"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>